<commit_message>
dev environment 20221103 1145
</commit_message>
<xml_diff>
--- a/Tickets/Normal Tickets/Ticket 33765/Test Plan.xlsx
+++ b/Tickets/Normal Tickets/Ticket 33765/Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\WIP\Tickets\Normal Tickets\Ticket 33765\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A3FE8-756A-4C5C-B304-C4A7A287ACCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6229D91-9B09-40A1-8123-9C71BC29124B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1815" windowWidth="23415" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="40" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>Test Case #</t>
   </si>
@@ -136,55 +136,64 @@
     <t>1) SQL Server Management Studio</t>
   </si>
   <si>
-    <t>Justin Pope - 11/2/2022</t>
-  </si>
-  <si>
     <t>Script in SQL Server Management Studio</t>
   </si>
   <si>
-    <t>1) Original Data
-Sales Order: 200-1070098
-2) Customer PO with GX prefix
-3) Customer PO with TEST prefix
-4) Customer PO with EB prefix
-5) Customer PO with CT prefix</t>
-  </si>
-  <si>
     <t>1) Original</t>
   </si>
   <si>
-    <t>2) CustomerPoNumber with GX prefix</t>
-  </si>
-  <si>
-    <t>3) CustomerPoNumber with TEST prefix</t>
-  </si>
-  <si>
-    <t>4) CustomerPoNumber with EB prefix</t>
-  </si>
-  <si>
-    <t>5) CustomerPoNumber with CT prefix</t>
-  </si>
-  <si>
     <t>Results below</t>
   </si>
   <si>
-    <t>Update Order Customer Po Number</t>
-  </si>
-  <si>
     <t>Edits in Syspro</t>
   </si>
   <si>
-    <t>2) Orders updated with exclusions</t>
-  </si>
-  <si>
-    <t>1) Original Data
-2) Sales Order: 301-1011380 Customer PO with GX prefix
-3) Sales Order: 260-1001112 Customer PO with TEST prefix
-4) Sales Order: 260-1001113 Customer PO with EB prefix
-5) Sales Order: 260-1001114 Customer PO with CT prefix</t>
-  </si>
-  <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>Original Data</t>
+  </si>
+  <si>
+    <t>Query Original TVF: tvf_RRS_CreditRequest()</t>
+  </si>
+  <si>
+    <t>Query Altered TVF: tvf_RRS_CreditRequest()</t>
+  </si>
+  <si>
+    <t>Alter CustomerPONumbers</t>
+  </si>
+  <si>
+    <t>Alter Data</t>
+  </si>
+  <si>
+    <t>Sales Order: 260-1001119 Customer PO with GX prefix
+Sales Order: 260-1001112 Customer PO with TEST prefix
+Sales Order: 260-1001113 Customer PO with EB prefix
+Sales Order: 260-1001114 Customer PO with CT prefix</t>
+  </si>
+  <si>
+    <t>Updated Data from Step 3</t>
+  </si>
+  <si>
+    <t>1) Original TVF</t>
+  </si>
+  <si>
+    <t>2) Altered TVF</t>
+  </si>
+  <si>
+    <t>4) Query After Alter</t>
+  </si>
+  <si>
+    <t>Query Original TVF: tvf_CIT_CreditRequest()</t>
+  </si>
+  <si>
+    <t>Query Altered TVF: tvf_CIT_CreditRequest()</t>
+  </si>
+  <si>
+    <t>2) Altered</t>
+  </si>
+  <si>
+    <t>Justin Pope - 11/3/2022</t>
   </si>
 </sst>
 </file>
@@ -313,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -399,6 +408,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -426,30 +444,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -458,12 +476,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,21 +500,21 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2335168</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>19550</xdr:rowOff>
+      <xdr:colOff>2563800</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>881</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3079FF64-4C0B-EF6B-488B-854F173FBF66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02D5B564-CEAE-FDEF-D990-1B043CFE2156}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -518,8 +530,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="809625" y="5724525"/>
-          <a:ext cx="11060068" cy="3581900"/>
+          <a:off x="809625" y="6534150"/>
+          <a:ext cx="11288700" cy="6315956"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -532,21 +544,21 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1258693</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>48264</xdr:rowOff>
+      <xdr:colOff>1754062</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>143822</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85A420FE-FE82-73FB-E9C5-AB1471E9CCCA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98AF7D7-B384-6222-722A-34534A1277AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -562,8 +574,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="809625" y="10096500"/>
-          <a:ext cx="9983593" cy="4582164"/>
+          <a:off x="809625" y="13173075"/>
+          <a:ext cx="10478962" cy="6782747"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1754062</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>105694</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC59362B-A071-A4B7-6620-E06B1313DC2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="20297775"/>
+          <a:ext cx="10478962" cy="6582694"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,21 +637,21 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>11664</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>152896</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>383021</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>86777</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{212A8C95-C35D-1C23-EA2E-E65D5B494DEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6493AE6-085C-F562-F7F6-173BA2215EC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -611,8 +667,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="809625" y="5400675"/>
-          <a:ext cx="15327864" cy="3553321"/>
+          <a:off x="809625" y="4914900"/>
+          <a:ext cx="14480021" cy="7535327"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -625,21 +681,21 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>221243</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>29393</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>154729</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>67679</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5507CD35-6F37-D34E-3939-BC0202E15868}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E302678D-9D54-46A2-D414-F2399F9C656B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -655,140 +711,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="809625" y="9286875"/>
-          <a:ext cx="15537443" cy="5858693"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>202191</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>114836</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81FF8A74-4E85-7117-FFC3-F87AC086FA9E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="809625" y="15601950"/>
-          <a:ext cx="15518391" cy="3839111"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>173612</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>475</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D231C6C-46EE-A4ED-A05A-3A4B0C6FC675}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="809625" y="19812000"/>
-          <a:ext cx="15489812" cy="3400900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>278401</xdr:colOff>
-      <xdr:row>151</xdr:row>
-      <xdr:rowOff>152873</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACCD7691-9EBE-AEB5-9A2E-7E3A301D75B0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="809625" y="23536275"/>
-          <a:ext cx="15594601" cy="3391373"/>
+          <a:off x="809625" y="12849225"/>
+          <a:ext cx="16690129" cy="7192379"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1124,7 +1048,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1091,7 @@
         <v>31</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.2">
@@ -1184,122 +1108,122 @@
         <v>31</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
+        <v>50</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
+        <v>50</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="29"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>1</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>2</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>3</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1330,11 +1254,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1345,62 +1269,64 @@
     <col min="4" max="4" width="42.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="42.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="42.42578125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="49.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="36">
+      <c r="B2" s="51"/>
+      <c r="C2" s="39">
         <v>1</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="36" t="str">
+      <c r="B3" s="51"/>
+      <c r="C3" s="39" t="str">
         <f>'Test Cases'!B2</f>
         <v>Test tvf_RRS_CreditRequest excludes pos with terms specified.</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="36" t="str">
+      <c r="B4" s="51"/>
+      <c r="C4" s="39" t="str">
         <f>'Test Cases'!D2</f>
         <v>1) SQL Server Management Studio</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="23" t="s">
         <v>19</v>
       </c>
@@ -1412,150 +1338,210 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-    </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="44">
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="43">
         <v>1</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="43">
+        <v>2</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="43">
+        <v>3</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="29" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="D9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="43">
+        <v>4</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="C10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-    </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40">
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="41">
         <v>1</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40">
-        <v>2</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-    </row>
-    <row r="12" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="16"/>
+      <c r="A13" s="41">
+        <v>2</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="26"/>
       <c r="D15" s="13"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="15"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
+      <c r="A16" s="47"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="47"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-    </row>
-    <row r="18" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C44" s="50" t="s">
-        <v>43</v>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="31"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C108" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A11:F11"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:F4"/>
@@ -1564,15 +1550,18 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1587,11 +1576,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD10"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1606,58 +1595,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="36">
+      <c r="B2" s="51"/>
+      <c r="C2" s="39">
         <v>2</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="36" t="str">
+      <c r="B3" s="51"/>
+      <c r="C3" s="39" t="str">
         <f>'Test Cases'!B3</f>
         <v>Test tvf_CIT_CreditRequest excludes pos with terms specified.</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="36" t="str">
+      <c r="B4" s="51"/>
+      <c r="C4" s="39" t="str">
         <f>'Test Cases'!D3</f>
         <v>1) SQL Server Management Studio</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="23" t="s">
         <v>19</v>
       </c>
@@ -1669,173 +1658,189 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-    </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="44">
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="43">
         <v>1</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="27" t="s">
-        <v>41</v>
+      <c r="B7" s="44"/>
+      <c r="C7" s="29" t="s">
+        <v>47</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="43">
+        <v>2</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-    </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40">
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41">
         <v>1</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40">
-        <v>2</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="28" t="s">
-        <v>42</v>
+      <c r="B10" s="42"/>
+      <c r="C10" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="41">
+        <v>2</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-    </row>
-    <row r="12" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
     </row>
     <row r="13" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="26"/>
       <c r="D15" s="13"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="15"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20"/>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-    </row>
-    <row r="18" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="49" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="49" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" s="49" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C108" s="49" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C131" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="19" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="30"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" s="30"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C109" s="30"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C132" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A17:F17"/>
+  <mergeCells count="21">
     <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A12:F12"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="C2:F2"/>

</xml_diff>